<commit_message>
feat: initialize react agent with engineering tools and configuration
</commit_message>
<xml_diff>
--- a/company_spreadsheets/AS_1720.1_2010_design_bending_capacity_formula_timber.xlsx
+++ b/company_spreadsheets/AS_1720.1_2010_design_bending_capacity_formula_timber.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>83333.33</v>
+        <v>83333</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>

</xml_diff>